<commit_message>
add functional radiobutton, need decision about choose of number button
</commit_message>
<xml_diff>
--- a/files/DownTime_shift.xlsx
+++ b/files/DownTime_shift.xlsx
@@ -388,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -960,17 +960,6 @@
       <top/>
       <bottom style="thin">
         <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1260,7 +1249,7 @@
     <xf applyAlignment="1" borderId="19" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="47" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="46" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="25" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1269,13 +1258,12 @@
     <xf applyAlignment="1" borderId="25" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="48" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="47" fillId="4" fontId="2" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="19" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="26" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="35" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1298,6 +1286,7 @@
     <xf applyAlignment="1" borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="32" fillId="4" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1311,7 +1300,7 @@
     <xf applyAlignment="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="46" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="4" fillId="7" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1624,7 +1613,7 @@
   <dimension ref="B4:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1658,11 +1647,11 @@
       <c r="N4" s="66" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="5" s="125" spans="1:17" thickBot="1">
-      <c r="B5" s="116" t="n"/>
-      <c r="C5" s="118" t="s">
+      <c r="B5" s="115" t="n"/>
+      <c r="C5" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="119" t="s">
+      <c r="D5" s="118" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="111" t="s">
@@ -1695,14 +1684,14 @@
       <c r="N5" s="66" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="6" s="125" spans="1:17" thickBot="1">
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="121">
+      <c r="C6" s="120">
         <f>main!J41</f>
         <v/>
       </c>
-      <c r="D6" s="122">
+      <c r="D6" s="121">
         <f>main!I40</f>
         <v/>
       </c>
@@ -1743,10 +1732,10 @@
       <c r="N6" s="66" t="n"/>
     </row>
     <row customHeight="1" ht="15.75" r="7" s="125" spans="1:17" thickBot="1">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="117">
+      <c r="C7" s="116">
         <f>main!N41</f>
         <v/>
       </c>
@@ -2147,7 +2136,7 @@
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -3478,10 +3467,10 @@
         <v>69</v>
       </c>
       <c r="B17" s="91" t="n">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C17" s="92" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D17" s="93" t="n">
         <v>0</v>
@@ -3490,7 +3479,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="93" t="n">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="G17" s="93" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
add check apl number, but write apl data to equipment file
</commit_message>
<xml_diff>
--- a/files/DownTime_shift.xlsx
+++ b/files/DownTime_shift.xlsx
@@ -1021,7 +1021,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="11" fillId="5" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1334,6 +1334,9 @@
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2161,7 +2164,7 @@
   <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -2318,49 +2321,49 @@
         <v>55</v>
       </c>
       <c r="B3" s="68" t="n">
-        <v>144</v>
+        <v>1</v>
       </c>
       <c r="C3" s="69" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D3" s="70" t="n">
-        <v>180</v>
+        <v>9</v>
       </c>
       <c r="E3" s="70" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F3" s="70" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="70" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="70" t="n">
         <v>10</v>
       </c>
-      <c r="G3" s="70" t="n">
-        <v>1086</v>
-      </c>
-      <c r="H3" s="70" t="n">
-        <v>49</v>
-      </c>
-      <c r="I3" s="70" t="n">
-        <v>8</v>
-      </c>
-      <c r="J3" s="71" t="n">
-        <v>14</v>
-      </c>
-      <c r="K3" s="69" t="n">
-        <v>66</v>
-      </c>
-      <c r="L3" s="70" t="n">
-        <v>40</v>
-      </c>
       <c r="M3" s="70" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N3" s="72" t="n">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="O3" s="73" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="P3" s="72" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="32">
         <f>SUM(B3:P3)</f>
@@ -2373,25 +2376,25 @@
         <v>0</v>
       </c>
       <c r="U3" s="78" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V3" s="78" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="W3" s="78" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="X3" s="78" t="n">
         <v>0</v>
       </c>
       <c r="Y3" s="89" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="78" t="n">
         <v>0</v>
       </c>
       <c r="AA3" s="79" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB3" s="32">
         <f>SUM(T3:AA3)</f>
@@ -2403,7 +2406,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="74" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="75" t="n">
         <v>0</v>
@@ -2488,7 +2491,7 @@
         <v>59</v>
       </c>
       <c r="B5" s="74" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="75" t="n">
         <v>0</v>
@@ -2573,7 +2576,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="74" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" s="75" t="n">
         <v>0</v>
@@ -2658,7 +2661,7 @@
         <v>63</v>
       </c>
       <c r="B7" s="74" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="75" t="n">
         <v>0</v>
@@ -2743,7 +2746,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="81" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C8" s="75" t="n">
         <v>0</v>
@@ -2828,7 +2831,7 @@
         <v>67</v>
       </c>
       <c r="B9" s="74" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C9" s="75" t="n">
         <v>0</v>
@@ -2913,7 +2916,7 @@
         <v>69</v>
       </c>
       <c r="B10" s="74" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C10" s="75" t="n">
         <v>0</v>
@@ -2998,7 +3001,7 @@
         <v>71</v>
       </c>
       <c r="B11" s="74" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C11" s="75" t="n">
         <v>0</v>
@@ -3083,7 +3086,7 @@
         <v>73</v>
       </c>
       <c r="B12" s="74" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C12" s="75" t="n">
         <v>0</v>
@@ -3168,7 +3171,7 @@
         <v>75</v>
       </c>
       <c r="B13" s="74" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13" s="75" t="n">
         <v>0</v>
@@ -3253,7 +3256,7 @@
         <v>77</v>
       </c>
       <c r="B14" s="74" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C14" s="83" t="n">
         <v>0</v>
@@ -3338,7 +3341,7 @@
         <v>79</v>
       </c>
       <c r="B15" s="74" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C15" s="75" t="n">
         <v>0</v>
@@ -3423,7 +3426,7 @@
         <v>81</v>
       </c>
       <c r="B16" s="74" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C16" s="75" t="n">
         <v>0</v>
@@ -3508,51 +3511,51 @@
         <v>83</v>
       </c>
       <c r="B17" s="84" t="n">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="C17" s="85" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="86" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E17" s="86" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F17" s="86" t="n">
-        <v>156</v>
+        <v>29</v>
       </c>
       <c r="G17" s="86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="86" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="I17" s="86" t="n">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="J17" s="87" t="n">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="K17" s="85" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="L17" s="86" t="n">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="M17" s="86" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N17" s="87" t="n">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="O17" s="88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P17" s="87" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="127">
         <f>SUM(B17:P17)</f>
         <v/>
       </c>
@@ -3599,28 +3602,28 @@
         <v>85</v>
       </c>
       <c r="T18" s="92" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="93" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V18" s="93" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W18" s="93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X18" s="93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y18" s="93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="32">
         <f>SUM(T18:AA18)</f>

</xml_diff>

<commit_message>
change logic in code
</commit_message>
<xml_diff>
--- a/files/DownTime_shift.xlsx
+++ b/files/DownTime_shift.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -1310,6 +1310,9 @@
     </xf>
     <xf borderId="31" fillId="0" fontId="11" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="14" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf applyAlignment="1" borderId="32" fillId="4" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1334,9 +1337,6 @@
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="14" fillId="0" fontId="7" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1638,43 +1638,43 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B4:Q25"/>
+  <dimension ref="A3:Q25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="119" width="5.7109375"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="119" width="17.42578125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="119" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="119" width="18.28515625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="119" width="17.85546875"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="119" width="9.42578125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="119" width="15.28515625"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="119" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="119" width="18.28515625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="119" width="9.42578125"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="119" width="15.28515625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="119" width="6.5703125"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="119" width="11"/>
+    <col customWidth="1" max="1" min="1" style="120" width="5.7109375"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="120" width="17.42578125"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="120" width="16.42578125"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="120" width="18.28515625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="120" width="17.85546875"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="120" width="9.42578125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="120" width="15.28515625"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="120" width="12.5703125"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="120" width="18.28515625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="120" width="9.42578125"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="120" width="15.28515625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="120" width="6.5703125"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="120" width="11"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="15.75" r="3" s="119" spans="1:17" thickBot="1"/>
-    <row customHeight="1" ht="15.75" r="4" s="119" spans="1:17" thickBot="1">
-      <c r="B4" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="122" t="s">
+    <row customHeight="1" ht="15.75" r="3" s="120" spans="1:17" thickBot="1"/>
+    <row customHeight="1" ht="15.75" r="4" s="120" spans="1:17" thickBot="1">
+      <c r="B4" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="123" t="s">
+      <c r="L4" s="124" t="s">
         <v>2</v>
       </c>
       <c r="N4" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="5" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="5" s="120" spans="1:17" thickBot="1">
       <c r="B5" s="108" t="n"/>
       <c r="C5" s="110" t="s">
         <v>3</v>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="N5" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="6" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="6" s="120" spans="1:17" thickBot="1">
       <c r="B6" s="112" t="s">
         <v>11</v>
       </c>
@@ -1723,15 +1723,15 @@
         <f>main!I40</f>
         <v/>
       </c>
-      <c r="E6" s="118">
+      <c r="E6" s="119">
         <f>main!Q40</f>
         <v/>
       </c>
-      <c r="F6" s="120">
+      <c r="F6" s="121">
         <f>E6/G6</f>
         <v/>
       </c>
-      <c r="G6" s="121" t="n">
+      <c r="G6" s="122" t="n">
         <v>7200</v>
       </c>
       <c r="H6" s="5">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="N6" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="7" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="7" s="120" spans="1:17" thickBot="1">
       <c r="B7" s="115" t="s">
         <v>12</v>
       </c>
@@ -1779,7 +1779,7 @@
       <c r="M7" s="98" t="n"/>
       <c r="N7" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="8" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="8" s="120" spans="1:17" thickBot="1">
       <c r="B8" s="36" t="n"/>
       <c r="G8" s="37" t="n"/>
       <c r="H8" s="36" t="n"/>
@@ -1790,7 +1790,7 @@
       <c r="N8" s="59" t="n"/>
       <c r="Q8" s="60" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="9" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="9" s="120" spans="1:17" thickBot="1">
       <c r="B9" s="36" t="n"/>
       <c r="D9" s="99" t="s">
         <v>9</v>
@@ -2080,7 +2080,7 @@
       <c r="K22" s="37" t="n"/>
       <c r="N22" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="23" s="119" spans="1:17">
+    <row customHeight="1" ht="15.75" r="23" s="120" spans="1:17">
       <c r="B23" s="36" t="n"/>
       <c r="C23" s="66" t="s">
         <v>27</v>
@@ -2101,7 +2101,7 @@
       <c r="K23" s="37" t="n"/>
       <c r="N23" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="24" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="24" s="120" spans="1:17" thickBot="1">
       <c r="B24" s="36" t="n"/>
       <c r="C24" s="67" t="s">
         <v>28</v>
@@ -2122,7 +2122,7 @@
       <c r="K24" s="37" t="n"/>
       <c r="N24" s="59" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="25" s="119" spans="1:17" thickBot="1">
+    <row customHeight="1" ht="15.75" r="25" s="120" spans="1:17" thickBot="1">
       <c r="B25" s="51" t="n"/>
       <c r="C25" s="52" t="n"/>
       <c r="D25" s="52" t="n"/>
@@ -2163,49 +2163,49 @@
   </sheetPr>
   <dimension ref="A1:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="119" width="11.28515625"/>
-    <col customWidth="1" max="2" min="2" style="119" width="10.7109375"/>
-    <col customWidth="1" max="3" min="3" style="119" width="9.28515625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="119" width="8.7109375"/>
-    <col customWidth="1" max="5" min="5" style="119" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="119" width="5.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="119" width="8.85546875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="119" width="6.42578125"/>
-    <col customWidth="1" max="9" min="9" style="119" width="9"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="119" width="8.140625"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="119" width="8.5703125"/>
-    <col customWidth="1" max="13" min="13" style="119" width="13.42578125"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="119" width="6"/>
-    <col customWidth="1" max="18" min="18" style="119" width="4"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" style="119" width="11.28515625"/>
-    <col customWidth="1" max="20" min="20" style="119" width="11"/>
-    <col customWidth="1" max="21" min="21" style="119" width="9.85546875"/>
-    <col customWidth="1" max="22" min="22" style="119" width="12.5703125"/>
-    <col customWidth="1" max="23" min="23" style="119" width="9.85546875"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" style="119" width="9"/>
-    <col customWidth="1" max="26" min="26" style="119" width="10.7109375"/>
-    <col customWidth="1" max="27" min="27" style="119" width="10.28515625"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" style="119" width="6"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="120" width="11.28515625"/>
+    <col customWidth="1" max="2" min="2" style="120" width="10.7109375"/>
+    <col customWidth="1" max="3" min="3" style="120" width="9.28515625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="120" width="8.7109375"/>
+    <col customWidth="1" max="5" min="5" style="120" width="10.5703125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="120" width="5.5703125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="120" width="8.85546875"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="120" width="6.42578125"/>
+    <col customWidth="1" max="9" min="9" style="120" width="9"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="120" width="8.140625"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="120" width="8.5703125"/>
+    <col customWidth="1" max="13" min="13" style="120" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="17" min="17" style="120" width="6"/>
+    <col customWidth="1" max="18" min="18" style="120" width="4"/>
+    <col bestFit="1" customWidth="1" max="19" min="19" style="120" width="11.28515625"/>
+    <col customWidth="1" max="20" min="20" style="120" width="11"/>
+    <col customWidth="1" max="21" min="21" style="120" width="9.85546875"/>
+    <col customWidth="1" max="22" min="22" style="120" width="12.5703125"/>
+    <col customWidth="1" max="23" min="23" style="120" width="9.85546875"/>
+    <col bestFit="1" customWidth="1" max="24" min="24" style="120" width="9"/>
+    <col customWidth="1" max="26" min="26" style="120" width="10.7109375"/>
+    <col customWidth="1" max="27" min="27" style="120" width="10.28515625"/>
+    <col bestFit="1" customWidth="1" max="28" min="28" style="120" width="6"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="39" r="1" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="39" r="1" s="120" spans="1:28" thickBot="1">
       <c r="A1" s="9" t="n"/>
       <c r="B1" s="10" t="n"/>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="125" t="s">
+      <c r="K1" s="126" t="s">
         <v>30</v>
       </c>
       <c r="O1" s="10" t="n"/>
       <c r="P1" s="10" t="n"/>
-      <c r="Q1" s="126" t="s">
+      <c r="Q1" s="127" t="s">
         <v>31</v>
       </c>
       <c r="S1" s="11" t="n"/>
@@ -2237,7 +2237,7 @@
         <v>31</v>
       </c>
     </row>
-    <row customHeight="1" ht="52.5" r="2" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="52.5" r="2" s="120" spans="1:28" thickBot="1">
       <c r="A2" s="16" t="n"/>
       <c r="B2" s="17" t="s">
         <v>40</v>
@@ -3506,7 +3506,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="17" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="15.75" r="17" s="120" spans="1:28" thickBot="1">
       <c r="A17" s="34" t="s">
         <v>83</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="87" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O17" s="88" t="n">
         <v>0</v>
@@ -3555,7 +3555,7 @@
       <c r="P17" s="87" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" s="127">
+      <c r="Q17" s="118">
         <f>SUM(B17:P17)</f>
         <v/>
       </c>
@@ -3591,7 +3591,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="18" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="15.75" r="18" s="120" spans="1:28" thickBot="1">
       <c r="A18" s="41" t="n"/>
       <c r="C18" s="36" t="n"/>
       <c r="J18" s="37" t="n"/>
@@ -3854,7 +3854,7 @@
       <c r="T38" s="36" t="n"/>
       <c r="AA38" s="37" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="39" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="15.75" r="39" s="120" spans="1:28" thickBot="1">
       <c r="C39" s="36" t="n"/>
       <c r="J39" s="37" t="n"/>
       <c r="K39" s="36" t="n"/>
@@ -3862,7 +3862,7 @@
       <c r="T39" s="36" t="n"/>
       <c r="AA39" s="37" t="n"/>
     </row>
-    <row customHeight="1" ht="16.5" r="40" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="16.5" r="40" s="120" spans="1:28" thickBot="1">
       <c r="A40" s="47" t="s">
         <v>86</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v/>
       </c>
     </row>
-    <row customHeight="1" ht="16.5" r="41" s="119" spans="1:28" thickBot="1">
+    <row customHeight="1" ht="16.5" r="41" s="120" spans="1:28" thickBot="1">
       <c r="C41" s="51" t="n"/>
       <c r="D41" s="52" t="n"/>
       <c r="E41" s="52" t="n"/>

</xml_diff>